<commit_message>
continuing to streamline dictionaries and working on Foundation Builder
</commit_message>
<xml_diff>
--- a/Building Blocks/Foundation_Builder.xlsx
+++ b/Building Blocks/Foundation_Builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\REEDR-O\Building Blocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1AA1A4-8482-4243-A61F-E5D75E12B988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C25F278-D02C-41A5-A710-26AF2183D5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28815" yWindow="15" windowWidth="14370" windowHeight="15555" xr2:uid="{D135BAC2-2A9D-498B-B692-4C5391A9D301}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D135BAC2-2A9D-498B-B692-4C5391A9D301}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,19 +36,145 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
   <si>
     <t>Vented Crawlspace - R0 Cavity Insulation</t>
   </si>
   <si>
     <t>Foundation Type</t>
+  </si>
+  <si>
+    <t>Vented Crawlspace</t>
+  </si>
+  <si>
+    <t>Interior Horizontal Insulation Material Name</t>
+  </si>
+  <si>
+    <t>Interior Vertical Insulation Material Name</t>
+  </si>
+  <si>
+    <t>Foundation And Floor Construction Name</t>
+  </si>
+  <si>
+    <t>Exterior Vertical Insulation Material Name</t>
+  </si>
+  <si>
+    <t>Vented Crawlspace - R13 Cavity Insulation</t>
+  </si>
+  <si>
+    <t>Vented Crawlspace - R19 Cavity Insulation</t>
+  </si>
+  <si>
+    <t>Vented Crawlspace - R30 Cavity Insulation</t>
+  </si>
+  <si>
+    <t>Vented Crawlspace - R38 Cavity Insulation</t>
+  </si>
+  <si>
+    <t>Slab - Uninsulated</t>
+  </si>
+  <si>
+    <t>Slab - R5 Perimeter with No Thermal Break</t>
+  </si>
+  <si>
+    <t>Slab - R5 Perimeter with R5 Thermal Break</t>
+  </si>
+  <si>
+    <t>Slab - R5 Under Full Slab with R5 Thermal Break</t>
+  </si>
+  <si>
+    <t>Slab - R10 Perimeter with No Thermal Break</t>
+  </si>
+  <si>
+    <t>Slab - R10 Perimeter with R5 Thermal Break</t>
+  </si>
+  <si>
+    <t>Slab - R10 Under Full Slab with R5 Thermal Break</t>
+  </si>
+  <si>
+    <t>Heated Basement - Uninsulated</t>
+  </si>
+  <si>
+    <t>Heated Basement - R5 Exterior Insulation</t>
+  </si>
+  <si>
+    <t>Heated Basement - R10 Exterior Insulation</t>
+  </si>
+  <si>
+    <t>Heated Basement - R15 Exterior Insulation</t>
+  </si>
+  <si>
+    <t>Unheated Basement - Uninsulated</t>
+  </si>
+  <si>
+    <t>Unheated Basement - R13 Cavity Insulation</t>
+  </si>
+  <si>
+    <t>Unheated Basement - R19 Cavity Insulation</t>
+  </si>
+  <si>
+    <t>Unheated Basement - R30 Cavity Insulation</t>
+  </si>
+  <si>
+    <t>Unheated Basement - R38 Cavity Insulation</t>
+  </si>
+  <si>
+    <t>Slab</t>
+  </si>
+  <si>
+    <t>Heated Basement</t>
+  </si>
+  <si>
+    <t>Unheated Basement</t>
+  </si>
+  <si>
+    <t>XPS_R5</t>
+  </si>
+  <si>
+    <t>Interior Horizontal Insulation Material Depth [ft]</t>
+  </si>
+  <si>
+    <t>Interior Horizontal Insulation Material Width [ft]</t>
+  </si>
+  <si>
+    <t>Interior Vertical Insulation Material Depth [ft]</t>
+  </si>
+  <si>
+    <t>Exterior Vertical Insulation Material Depth [ft]</t>
+  </si>
+  <si>
+    <t>Foundation Wall Height Above Grade [ft]</t>
+  </si>
+  <si>
+    <t>Foundation Wall Height Below Slab [ft]</t>
+  </si>
+  <si>
+    <t>Floor Insulation Layer Material Name</t>
+  </si>
+  <si>
+    <t>Fiberglass_Batt_R0</t>
+  </si>
+  <si>
+    <t>Fiberglass_Batt_R13</t>
+  </si>
+  <si>
+    <t>Fiberglass_Batt_R19</t>
+  </si>
+  <si>
+    <t>Fiberglass_Batt_R30</t>
+  </si>
+  <si>
+    <t>Fiberglass_Batt_R38</t>
+  </si>
+  <si>
+    <t>XPS_R10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +200,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -95,15 +227,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -419,143 +560,530 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92667E3-9923-4324-8BDC-0F2F184C447E}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="44.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="16.5703125" style="1" customWidth="1"/>
+    <col min="6" max="8" width="15.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="1" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K2" s="4">
+        <v>1</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K5" s="4">
+        <v>1</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>2</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="2"/>
     </row>
@@ -576,6 +1104,12 @@
       <c r="B36" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B22" xr:uid="{215A9823-175F-4791-911E-FBBBBEE8A6A6}">
+      <formula1>"Vented Crawlspace, Slab, Heated Basement, Unheated Basement"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>